<commit_message>
add staff team site creation
</commit_message>
<xml_diff>
--- a/Fast Deploy Microsoft Teams for Education.xlsx
+++ b/Fast Deploy Microsoft Teams for Education.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdowst\Desktop\EdTeams\School-Hydration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D01927-3827-4311-883A-7C89CF733AC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD4DD13-0A5C-4969-A61C-A1858A7C0277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7C5A87EF-6C76-49E3-93EB-E3C4DB0EE31A}"/>
+    <workbookView xWindow="5250" yWindow="2250" windowWidth="18900" windowHeight="10980" xr2:uid="{7C5A87EF-6C76-49E3-93EB-E3C4DB0EE31A}"/>
   </bookViews>
   <sheets>
     <sheet name="School Details" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="527">
   <si>
     <t>Teachers</t>
   </si>
@@ -60,12 +60,6 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>Jill</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
     <t>Classes</t>
   </si>
   <si>
@@ -78,66 +72,6 @@
     <t>Class Name</t>
   </si>
   <si>
-    <t>Jeff</t>
-  </si>
-  <si>
-    <t>Read</t>
-  </si>
-  <si>
-    <t>Phyllis</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Carl</t>
-  </si>
-  <si>
-    <t>Davis</t>
-  </si>
-  <si>
-    <t>Barbara</t>
-  </si>
-  <si>
-    <t>Bell</t>
-  </si>
-  <si>
-    <t>Catherine</t>
-  </si>
-  <si>
-    <t>Rivera</t>
-  </si>
-  <si>
-    <t>Edward</t>
-  </si>
-  <si>
-    <t>Jackson</t>
-  </si>
-  <si>
-    <t>Intro to College Algebra</t>
-  </si>
-  <si>
-    <t>Jill Smith - S0001</t>
-  </si>
-  <si>
-    <t>Jeff Read - T0001</t>
-  </si>
-  <si>
-    <t>Carl Davis - S0002</t>
-  </si>
-  <si>
-    <t>Phyllis Price - T0002</t>
-  </si>
-  <si>
-    <t>Barbara Bell - S0003</t>
-  </si>
-  <si>
-    <t>Edward Jackson - S0005</t>
-  </si>
-  <si>
-    <t>Chemistry</t>
-  </si>
-  <si>
     <t>Fast Deploy Microsoft Teams for Education</t>
   </si>
   <si>
@@ -151,9 +85,6 @@
   </si>
   <si>
     <t>Envelope is in this cell</t>
-  </si>
-  <si>
-    <t>Enter your school name here</t>
   </si>
   <si>
     <t>Naming Pattern:</t>
@@ -1733,10 +1664,10 @@
     </r>
   </si>
   <si>
-    <t>Catherine Rivera - S0004</t>
-  </si>
-  <si>
     <t>Note: The Start-Upload.bat is deisgned to run multiple times, without adding duplicates. So, if you add additional students, teachers, or classes to this workbook, then you can simpily run the Start-Upload.bat again.</t>
+  </si>
+  <si>
+    <t>Enter your school name here</t>
   </si>
 </sst>
 </file>
@@ -2033,15 +1964,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2068,6 +1990,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -3109,124 +3040,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="2:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="B2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="2:5" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>36</v>
+      <c r="B3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="20"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="21"/>
-      <c r="C5" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>38</v>
+      <c r="B5" s="18"/>
+      <c r="C5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="20"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>517</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>495</v>
-      </c>
-      <c r="E7" s="12" t="str">
+      <c r="B7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>472</v>
+      </c>
+      <c r="E7" s="21" t="str">
         <f>VLOOKUP(D7,List!$C$2:$D$250,2,FALSE)</f>
         <v>US</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="10" spans="2:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
-        <v>545</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="B10" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="2:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
-        <v>546</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
+      <c r="B11" s="12" t="s">
+        <v>523</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="2:5" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
-        <v>547</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="B12" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>543</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
-        <v>544</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="2:5" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
-        <v>549</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="B15" s="20" t="s">
+        <v>525</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D7:D8"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B3:B4"/>
@@ -3237,9 +3169,8 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter personal details in cells C3 through E8 and Insurance information in cells H3 through K8" sqref="B3:B5" xr:uid="{AE09E1FE-0AE1-454D-B77A-CBFD565068BC}"/>
@@ -3300,7 +3231,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="8" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2"/>
     </row>
@@ -3315,7 +3246,7 @@
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>3</v>
@@ -3324,39 +3255,27 @@
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f t="shared" ref="B4:B67" si="0">IF(ISBLANK(C4),"","T" &amp; TEXT(ROW()-3,"0000"))</f>
-        <v>T0001</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
+        <v/>
       </c>
       <c r="E4" t="str">
         <f>IF(ISBLANK(C4),"",TRIM(C4) &amp; " " &amp; TRIM(D4) &amp; " - " &amp; B4)</f>
-        <v>Jeff Read - T0001</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>T0002</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
+        <v/>
       </c>
       <c r="E5" t="str">
         <f t="shared" ref="E5:E67" si="1">IF(ISBLANK(C5),"",TRIM(C5) &amp; " " &amp; TRIM(D5) &amp; " - " &amp; B5)</f>
-        <v>Phyllis Price - T0002</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -11223,7 +11142,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="8" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2"/>
     </row>
@@ -11247,87 +11166,57 @@
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f t="shared" ref="B4:B67" si="0">IF(ISBLANK(C4),"","S" &amp; TEXT(ROW()-3,"0000"))</f>
-        <v>S0001</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
+        <v/>
       </c>
       <c r="E4" t="str">
         <f t="shared" ref="E4:E67" si="1">IF(ISBLANK(C4),"",TRIM(C4) &amp; " " &amp; TRIM(D4) &amp; " - " &amp; B4)</f>
-        <v>Jill Smith - S0001</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>S0002</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v/>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>Carl Davis - S0002</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>S0003</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
+        <v/>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>Barbara Bell - S0003</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>S0004</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
+        <v/>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>Catherine Rivera - S0004</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>S0005</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
+        <v/>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>Edward Jackson - S0005</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -19163,20 +19052,20 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="8" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -19185,82 +19074,49 @@
         <v>1</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="str">
+      <c r="E4">
         <f>B4</f>
-        <v>Intro to College Algebra</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
       <c r="E5" t="str">
         <f>IF(AND(ISBLANK(C5),ISBLANK(D5)),"",IF(ISBLANK(B5),E4,B5))</f>
-        <v>Intro to College Algebra</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" t="str">
         <f t="shared" ref="E6:E69" si="0">IF(AND(ISBLANK(C6),ISBLANK(D6)),"",IF(ISBLANK(B6),E5,B6))</f>
-        <v>Intro to College Algebra</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>Intro to College Algebra</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>Chemistry</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>548</v>
-      </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>Chemistry</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>Chemistry</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -23967,2011 +23823,2011 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>542</v>
+        <v>519</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>541</v>
+        <v>518</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>540</v>
+        <v>517</v>
       </c>
       <c r="D35" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>539</v>
+        <v>516</v>
       </c>
       <c r="D39" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="D41" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="D42" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="D43" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="D45" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="D46" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D49" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="D51" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="D52" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>538</v>
+        <v>515</v>
       </c>
       <c r="D53" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="D54" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="D55" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>537</v>
+        <v>514</v>
       </c>
       <c r="D56" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="D58" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="D59" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="D60" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="D61" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="D62" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="D64" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="D65" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="D66" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="D67" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="D68" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="D69" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="D70" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="D71" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>536</v>
+        <v>513</v>
       </c>
       <c r="D72" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="D73" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>535</v>
+        <v>512</v>
       </c>
       <c r="D74" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="D75" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="D76" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="D77" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="D78" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="D79" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="D80" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>534</v>
+        <v>511</v>
       </c>
       <c r="D81" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="D82" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="D83" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="D84" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="D85" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="D86" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="D87" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="D88" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="D89" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="D90" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="D91" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="D92" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="D93" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="D94" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="D95" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
     </row>
     <row r="96" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="D96" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="D97" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="D98" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
     </row>
     <row r="99" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="D99" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
     </row>
     <row r="100" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C100" t="s">
-        <v>533</v>
+        <v>510</v>
       </c>
       <c r="D100" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="D101" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
     </row>
     <row r="102" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C102" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="D102" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="D103" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
     </row>
     <row r="104" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="D104" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="D105" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
     </row>
     <row r="106" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="D106" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
     </row>
     <row r="107" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="D107" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
     </row>
     <row r="108" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="D108" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
     </row>
     <row r="109" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C109" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="D109" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
     </row>
     <row r="110" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
       <c r="D110" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
     </row>
     <row r="111" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="D111" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
     </row>
     <row r="112" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="D112" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
     </row>
     <row r="113" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C113" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
       <c r="D113" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
     </row>
     <row r="114" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C114" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="D114" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
     </row>
     <row r="115" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="D115" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
     </row>
     <row r="116" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C116" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
       <c r="D116" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
     </row>
     <row r="117" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="D117" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
     </row>
     <row r="118" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C118" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="D118" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
     </row>
     <row r="119" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="D119" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C120" t="s">
-        <v>532</v>
+        <v>509</v>
       </c>
       <c r="D120" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
     </row>
     <row r="121" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="D121" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
     </row>
     <row r="122" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="D122" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
     </row>
     <row r="123" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="D123" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
     </row>
     <row r="124" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
-        <v>531</v>
+        <v>508</v>
       </c>
       <c r="D124" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="D125" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
     </row>
     <row r="126" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="D126" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="D127" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
     </row>
     <row r="128" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="D128" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
     </row>
     <row r="129" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C129" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="D129" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
     </row>
     <row r="130" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C130" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="D130" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
     </row>
     <row r="131" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="D131" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
     </row>
     <row r="132" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C132" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="D132" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
     </row>
     <row r="133" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C133" t="s">
-        <v>530</v>
+        <v>507</v>
       </c>
       <c r="D133" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
     </row>
     <row r="134" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C134" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="D134" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
     </row>
     <row r="135" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="D135" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
     </row>
     <row r="136" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C136" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="D136" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
     </row>
     <row r="137" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
-        <v>301</v>
+        <v>278</v>
       </c>
       <c r="D137" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
     </row>
     <row r="138" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
-        <v>303</v>
+        <v>280</v>
       </c>
       <c r="D138" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
     </row>
     <row r="139" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="D139" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
     </row>
     <row r="140" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
       <c r="D140" t="s">
-        <v>308</v>
+        <v>285</v>
       </c>
     </row>
     <row r="141" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C141" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="D141" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
     </row>
     <row r="142" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C142" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
       <c r="D142" t="s">
-        <v>312</v>
+        <v>289</v>
       </c>
     </row>
     <row r="143" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
-        <v>313</v>
+        <v>290</v>
       </c>
       <c r="D143" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
     </row>
     <row r="144" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C144" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="D144" t="s">
-        <v>316</v>
+        <v>293</v>
       </c>
     </row>
     <row r="145" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C145" t="s">
-        <v>317</v>
+        <v>294</v>
       </c>
       <c r="D145" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
     </row>
     <row r="146" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C146" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
       <c r="D146" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
     </row>
     <row r="147" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C147" t="s">
-        <v>321</v>
+        <v>298</v>
       </c>
       <c r="D147" t="s">
-        <v>322</v>
+        <v>299</v>
       </c>
     </row>
     <row r="148" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C148" t="s">
-        <v>323</v>
+        <v>300</v>
       </c>
       <c r="D148" t="s">
-        <v>324</v>
+        <v>301</v>
       </c>
     </row>
     <row r="149" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C149" t="s">
-        <v>325</v>
+        <v>302</v>
       </c>
       <c r="D149" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
     </row>
     <row r="150" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C150" t="s">
-        <v>327</v>
+        <v>304</v>
       </c>
       <c r="D150" t="s">
-        <v>328</v>
+        <v>305</v>
       </c>
     </row>
     <row r="151" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C151" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="D151" t="s">
-        <v>330</v>
+        <v>307</v>
       </c>
     </row>
     <row r="152" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
-        <v>331</v>
+        <v>308</v>
       </c>
       <c r="D152" t="s">
-        <v>332</v>
+        <v>309</v>
       </c>
     </row>
     <row r="153" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>333</v>
+        <v>310</v>
       </c>
       <c r="D153" t="s">
-        <v>334</v>
+        <v>311</v>
       </c>
     </row>
     <row r="154" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
-        <v>529</v>
+        <v>506</v>
       </c>
       <c r="D154" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
     </row>
     <row r="155" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="D155" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
     </row>
     <row r="156" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
       <c r="D156" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
     </row>
     <row r="157" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="D157" t="s">
-        <v>341</v>
+        <v>318</v>
       </c>
     </row>
     <row r="158" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="D158" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
     </row>
     <row r="159" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C159" t="s">
-        <v>344</v>
+        <v>321</v>
       </c>
       <c r="D159" t="s">
-        <v>345</v>
+        <v>322</v>
       </c>
     </row>
     <row r="160" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>346</v>
+        <v>323</v>
       </c>
       <c r="D160" t="s">
-        <v>347</v>
+        <v>324</v>
       </c>
     </row>
     <row r="161" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
-        <v>348</v>
+        <v>325</v>
       </c>
       <c r="D161" t="s">
-        <v>349</v>
+        <v>326</v>
       </c>
     </row>
     <row r="162" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
-        <v>350</v>
+        <v>327</v>
       </c>
       <c r="D162" t="s">
-        <v>351</v>
+        <v>328</v>
       </c>
     </row>
     <row r="163" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
-        <v>352</v>
+        <v>329</v>
       </c>
       <c r="D163" t="s">
-        <v>353</v>
+        <v>330</v>
       </c>
     </row>
     <row r="164" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="D164" t="s">
-        <v>355</v>
+        <v>332</v>
       </c>
     </row>
     <row r="165" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C165" t="s">
-        <v>356</v>
+        <v>333</v>
       </c>
       <c r="D165" t="s">
-        <v>357</v>
+        <v>334</v>
       </c>
     </row>
     <row r="166" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C166" t="s">
-        <v>528</v>
+        <v>505</v>
       </c>
       <c r="D166" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
     </row>
     <row r="167" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C167" t="s">
-        <v>359</v>
+        <v>336</v>
       </c>
       <c r="D167" t="s">
-        <v>360</v>
+        <v>337</v>
       </c>
     </row>
     <row r="168" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C168" t="s">
-        <v>361</v>
+        <v>338</v>
       </c>
       <c r="D168" t="s">
-        <v>362</v>
+        <v>339</v>
       </c>
     </row>
     <row r="169" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C169" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
       <c r="D169" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
     </row>
     <row r="170" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C170" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="D170" t="s">
-        <v>366</v>
+        <v>343</v>
       </c>
     </row>
     <row r="171" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C171" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="D171" t="s">
-        <v>368</v>
+        <v>345</v>
       </c>
     </row>
     <row r="172" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C172" t="s">
-        <v>369</v>
+        <v>346</v>
       </c>
       <c r="D172" t="s">
-        <v>370</v>
+        <v>347</v>
       </c>
     </row>
     <row r="173" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C173" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="D173" t="s">
-        <v>372</v>
+        <v>349</v>
       </c>
     </row>
     <row r="174" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C174" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="D174" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
     </row>
     <row r="175" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C175" t="s">
-        <v>375</v>
+        <v>352</v>
       </c>
       <c r="D175" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
     </row>
     <row r="176" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C176" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
       <c r="D176" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
     </row>
     <row r="177" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C177" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="D177" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
     </row>
     <row r="178" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C178" t="s">
-        <v>527</v>
+        <v>504</v>
       </c>
       <c r="D178" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
     </row>
     <row r="179" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C179" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="D179" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
     </row>
     <row r="180" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C180" t="s">
-        <v>384</v>
+        <v>361</v>
       </c>
       <c r="D180" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
     </row>
     <row r="181" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C181" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="D181" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
     </row>
     <row r="182" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C182" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="D182" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
     </row>
     <row r="183" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C183" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="D183" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
     </row>
     <row r="184" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C184" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
       <c r="D184" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
     </row>
     <row r="185" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C185" t="s">
-        <v>526</v>
+        <v>503</v>
       </c>
       <c r="D185" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
     </row>
     <row r="186" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C186" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="D186" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
     </row>
     <row r="187" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C187" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="D187" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
     </row>
     <row r="188" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C188" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="D188" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
     </row>
     <row r="189" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C189" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
       <c r="D189" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
     </row>
     <row r="190" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C190" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="D190" t="s">
-        <v>404</v>
+        <v>381</v>
       </c>
     </row>
     <row r="191" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C191" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="D191" t="s">
-        <v>406</v>
+        <v>383</v>
       </c>
     </row>
     <row r="192" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C192" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="D192" t="s">
-        <v>408</v>
+        <v>385</v>
       </c>
     </row>
     <row r="193" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C193" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="D193" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
     </row>
     <row r="194" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C194" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
       <c r="D194" t="s">
-        <v>412</v>
+        <v>389</v>
       </c>
     </row>
     <row r="195" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C195" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
       <c r="D195" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
     </row>
     <row r="196" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C196" t="s">
-        <v>415</v>
+        <v>392</v>
       </c>
       <c r="D196" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
     </row>
     <row r="197" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C197" t="s">
-        <v>417</v>
+        <v>394</v>
       </c>
       <c r="D197" t="s">
-        <v>418</v>
+        <v>395</v>
       </c>
     </row>
     <row r="198" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C198" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
       <c r="D198" t="s">
-        <v>420</v>
+        <v>397</v>
       </c>
     </row>
     <row r="199" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C199" t="s">
-        <v>421</v>
+        <v>398</v>
       </c>
       <c r="D199" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
     </row>
     <row r="200" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C200" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="D200" t="s">
-        <v>424</v>
+        <v>401</v>
       </c>
     </row>
     <row r="201" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C201" t="s">
-        <v>425</v>
+        <v>402</v>
       </c>
       <c r="D201" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
     </row>
     <row r="202" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C202" t="s">
-        <v>427</v>
+        <v>404</v>
       </c>
       <c r="D202" t="s">
-        <v>428</v>
+        <v>405</v>
       </c>
     </row>
     <row r="203" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C203" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="D203" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
     </row>
     <row r="204" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C204" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="D204" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
     </row>
     <row r="205" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C205" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="D205" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
     </row>
     <row r="206" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C206" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="D206" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
     </row>
     <row r="207" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C207" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="D207" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
     </row>
     <row r="208" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C208" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="D208" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
     </row>
     <row r="209" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C209" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
       <c r="D209" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
     </row>
     <row r="210" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C210" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
       <c r="D210" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
     </row>
     <row r="211" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C211" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
       <c r="D211" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
     </row>
     <row r="212" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C212" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="D212" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
     </row>
     <row r="213" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C213" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
       <c r="D213" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
     </row>
     <row r="214" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C214" t="s">
-        <v>451</v>
+        <v>428</v>
       </c>
       <c r="D214" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
     </row>
     <row r="215" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C215" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="D215" t="s">
-        <v>454</v>
+        <v>431</v>
       </c>
     </row>
     <row r="216" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C216" t="s">
-        <v>455</v>
+        <v>432</v>
       </c>
       <c r="D216" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
     </row>
     <row r="217" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C217" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="D217" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
     </row>
     <row r="218" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C218" t="s">
-        <v>525</v>
+        <v>502</v>
       </c>
       <c r="D218" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
     </row>
     <row r="219" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C219" t="s">
-        <v>524</v>
+        <v>501</v>
       </c>
       <c r="D219" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
     </row>
     <row r="220" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C220" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
       <c r="D220" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
     </row>
     <row r="221" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C221" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="D221" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
     </row>
     <row r="222" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C222" t="s">
-        <v>465</v>
+        <v>442</v>
       </c>
       <c r="D222" t="s">
-        <v>466</v>
+        <v>443</v>
       </c>
     </row>
     <row r="223" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C223" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
       <c r="D223" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
     </row>
     <row r="224" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C224" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
       <c r="D224" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
     </row>
     <row r="225" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C225" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
       <c r="D225" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
     </row>
     <row r="226" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C226" t="s">
-        <v>472</v>
+        <v>449</v>
       </c>
       <c r="D226" t="s">
-        <v>473</v>
+        <v>450</v>
       </c>
     </row>
     <row r="227" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C227" t="s">
-        <v>474</v>
+        <v>451</v>
       </c>
       <c r="D227" t="s">
-        <v>475</v>
+        <v>452</v>
       </c>
     </row>
     <row r="228" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C228" t="s">
-        <v>476</v>
+        <v>453</v>
       </c>
       <c r="D228" t="s">
-        <v>477</v>
+        <v>454</v>
       </c>
     </row>
     <row r="229" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C229" t="s">
-        <v>478</v>
+        <v>455</v>
       </c>
       <c r="D229" t="s">
-        <v>479</v>
+        <v>456</v>
       </c>
     </row>
     <row r="230" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C230" t="s">
-        <v>480</v>
+        <v>457</v>
       </c>
       <c r="D230" t="s">
-        <v>481</v>
+        <v>458</v>
       </c>
     </row>
     <row r="231" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C231" t="s">
-        <v>482</v>
+        <v>459</v>
       </c>
       <c r="D231" t="s">
-        <v>483</v>
+        <v>460</v>
       </c>
     </row>
     <row r="232" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C232" t="s">
-        <v>484</v>
+        <v>461</v>
       </c>
       <c r="D232" t="s">
-        <v>485</v>
+        <v>462</v>
       </c>
     </row>
     <row r="233" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C233" t="s">
-        <v>486</v>
+        <v>463</v>
       </c>
       <c r="D233" t="s">
-        <v>487</v>
+        <v>464</v>
       </c>
     </row>
     <row r="234" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C234" t="s">
-        <v>488</v>
+        <v>465</v>
       </c>
       <c r="D234" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
     </row>
     <row r="235" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C235" t="s">
-        <v>490</v>
+        <v>467</v>
       </c>
       <c r="D235" t="s">
-        <v>491</v>
+        <v>468</v>
       </c>
     </row>
     <row r="236" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C236" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
       <c r="D236" t="s">
-        <v>493</v>
+        <v>470</v>
       </c>
     </row>
     <row r="237" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C237" t="s">
-        <v>522</v>
+        <v>499</v>
       </c>
       <c r="D237" t="s">
-        <v>494</v>
+        <v>471</v>
       </c>
     </row>
     <row r="238" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C238" t="s">
-        <v>495</v>
+        <v>472</v>
       </c>
       <c r="D238" t="s">
-        <v>496</v>
+        <v>473</v>
       </c>
     </row>
     <row r="239" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C239" t="s">
-        <v>497</v>
+        <v>474</v>
       </c>
       <c r="D239" t="s">
-        <v>498</v>
+        <v>475</v>
       </c>
     </row>
     <row r="240" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C240" t="s">
-        <v>499</v>
+        <v>476</v>
       </c>
       <c r="D240" t="s">
-        <v>500</v>
+        <v>477</v>
       </c>
     </row>
     <row r="241" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C241" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
       <c r="D241" t="s">
-        <v>502</v>
+        <v>479</v>
       </c>
     </row>
     <row r="242" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C242" t="s">
-        <v>503</v>
+        <v>480</v>
       </c>
       <c r="D242" t="s">
-        <v>504</v>
+        <v>481</v>
       </c>
     </row>
     <row r="243" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C243" t="s">
-        <v>521</v>
+        <v>498</v>
       </c>
       <c r="D243" t="s">
-        <v>505</v>
+        <v>482</v>
       </c>
     </row>
     <row r="244" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C244" t="s">
-        <v>520</v>
+        <v>497</v>
       </c>
       <c r="D244" t="s">
-        <v>506</v>
+        <v>483</v>
       </c>
     </row>
     <row r="245" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C245" t="s">
-        <v>518</v>
+        <v>495</v>
       </c>
       <c r="D245" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
     </row>
     <row r="246" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C246" t="s">
-        <v>508</v>
+        <v>485</v>
       </c>
       <c r="D246" t="s">
-        <v>509</v>
+        <v>486</v>
       </c>
     </row>
     <row r="247" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C247" t="s">
-        <v>519</v>
+        <v>496</v>
       </c>
       <c r="D247" t="s">
-        <v>510</v>
+        <v>487</v>
       </c>
     </row>
     <row r="248" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C248" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
       <c r="D248" t="s">
-        <v>512</v>
+        <v>489</v>
       </c>
     </row>
     <row r="249" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C249" t="s">
-        <v>513</v>
+        <v>490</v>
       </c>
       <c r="D249" t="s">
-        <v>514</v>
+        <v>491</v>
       </c>
     </row>
     <row r="250" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C250" t="s">
-        <v>515</v>
+        <v>492</v>
       </c>
       <c r="D250" t="s">
-        <v>516</v>
+        <v>493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>